<commit_message>
Work log and time update
</commit_message>
<xml_diff>
--- a/BoardGame/Stephanie.xlsx
+++ b/BoardGame/Stephanie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ng6739fk/Documents/GitHub/410/BoardGame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6441FF8-1EEB-194C-BDAB-B6277CE506C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2688F81-57F1-E441-9AEA-455CC125A8CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1960" yWindow="1140" windowWidth="16160" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -133,10 +133,10 @@
     <t>2 hours</t>
   </si>
   <si>
-    <t>2.5 hours</t>
-  </si>
-  <si>
     <t>1 hour drawing a picture</t>
+  </si>
+  <si>
+    <t>3.5 hours</t>
   </si>
 </sst>
 </file>
@@ -1069,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1191,7 +1191,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -1217,7 +1217,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>

</xml_diff>

<commit_message>
Get current turn and matrix from match/game
Also changed g to game
</commit_message>
<xml_diff>
--- a/BoardGame/Stephanie.xlsx
+++ b/BoardGame/Stephanie.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ng6739fk/Documents/GitHub/410/BoardGame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2688F81-57F1-E441-9AEA-455CC125A8CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D120CD-F12E-6F47-B184-71E01FEC0881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1960" yWindow="1140" windowWidth="16160" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,7 +136,7 @@
     <t>1 hour drawing a picture</t>
   </si>
   <si>
-    <t>3.5 hours</t>
+    <t>4.5 hours</t>
   </si>
 </sst>
 </file>
@@ -1069,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Filled out excel document
</commit_message>
<xml_diff>
--- a/BoardGame/Stephanie.xlsx
+++ b/BoardGame/Stephanie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ng6739fk/Documents/GitHub/410/BoardGame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D120CD-F12E-6F47-B184-71E01FEC0881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F813487A-17BB-A841-8090-129B65C2D54B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="1140" windowWidth="16160" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="720" windowWidth="27020" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Copyright - Sudharsan Iyengar - August 2017.</t>
   </si>
@@ -97,12 +97,6 @@
     <t>Tracking Project Work</t>
   </si>
   <si>
-    <t>Team Name:</t>
-  </si>
-  <si>
-    <t>Total time Spent</t>
-  </si>
-  <si>
     <t>Member Contribution</t>
   </si>
   <si>
@@ -112,9 +106,6 @@
     <t>Component Name</t>
   </si>
   <si>
-    <t>Total time spent on component</t>
-  </si>
-  <si>
     <t>General Description of Components</t>
   </si>
   <si>
@@ -130,13 +121,88 @@
     <t>Team Members responsible</t>
   </si>
   <si>
-    <t>2 hours</t>
-  </si>
-  <si>
-    <t>1 hour drawing a picture</t>
-  </si>
-  <si>
-    <t>4.5 hours</t>
+    <t>Bored Game</t>
+  </si>
+  <si>
+    <t>Spaghetti Monster Acolytes</t>
+  </si>
+  <si>
+    <t>Team Name: T3, aka</t>
+  </si>
+  <si>
+    <t>12 hours</t>
+  </si>
+  <si>
+    <t>100+ times</t>
+  </si>
+  <si>
+    <t>see gitHub</t>
+  </si>
+  <si>
+    <t>4 hours sketching diagrams</t>
+  </si>
+  <si>
+    <t>32.0 hours</t>
+  </si>
+  <si>
+    <t>10 times</t>
+  </si>
+  <si>
+    <t>4 hours</t>
+  </si>
+  <si>
+    <t>15 times</t>
+  </si>
+  <si>
+    <t>30 times</t>
+  </si>
+  <si>
+    <t>20+ times</t>
+  </si>
+  <si>
+    <t>camaraderie</t>
+  </si>
+  <si>
+    <t>95 (lacking sanitation and error recovery)</t>
+  </si>
+  <si>
+    <t>90 (could always use more testing)</t>
+  </si>
+  <si>
+    <t>Adam Stammer</t>
+  </si>
+  <si>
+    <t>Henry Weber</t>
+  </si>
+  <si>
+    <t>Stephanie Smith</t>
+  </si>
+  <si>
+    <t>Akin Tema-Lopez</t>
+  </si>
+  <si>
+    <t>Network Handler</t>
+  </si>
+  <si>
+    <t>Gui</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>Match</t>
+  </si>
+  <si>
+    <t>total 53 hours</t>
+  </si>
+  <si>
+    <t>1 hours talking about it after testing</t>
+  </si>
+  <si>
+    <t>Total time spent on component (hours)</t>
+  </si>
+  <si>
+    <t>Total time Spent (hours)</t>
   </si>
 </sst>
 </file>
@@ -1067,15 +1133,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M16"/>
+  <dimension ref="B1:M17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="1" customWidth="1"/>
     <col min="4" max="5" width="14.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.1640625" style="1" customWidth="1"/>
@@ -1102,24 +1168,29 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="2:13">
+    <row r="4" spans="2:13" ht="32">
       <c r="C4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
-        <v>25</v>
-      </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:13">
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="2:13" ht="48">
+      <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="64">
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1136,17 +1207,17 @@
         <v>6</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1165,15 +1236,29 @@
         <v>7</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
+        <v>40</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="8">
+        <v>100</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="11">
+        <v>24.25</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M8" s="11">
+        <v>7.25</v>
+      </c>
     </row>
     <row r="9" spans="2:13">
       <c r="C9" s="7"/>
@@ -1186,20 +1271,34 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="2:13" ht="48">
+    <row r="10" spans="2:13" ht="48" customHeight="1">
       <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="8">
+        <v>100</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="11">
+        <v>8.75</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" s="11">
+        <v>21.25</v>
+      </c>
     </row>
     <row r="11" spans="2:13">
       <c r="C11" s="7"/>
@@ -1217,15 +1316,29 @@
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
+      <c r="G12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="11">
+        <v>11.25</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12" s="11">
+        <v>11.25</v>
+      </c>
     </row>
     <row r="13" spans="2:13">
       <c r="C13" s="7"/>
@@ -1238,18 +1351,34 @@
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="2:13" ht="32">
+    <row r="14" spans="2:13" ht="48">
       <c r="C14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
+      <c r="D14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="11">
+        <v>5.75</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" s="11">
+        <v>13.25</v>
+      </c>
     </row>
     <row r="15" spans="2:13">
       <c r="C15" s="7"/>
@@ -1266,10 +1395,26 @@
       <c r="C16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="8">
+        <v>100</v>
+      </c>
+      <c r="M16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" ht="16">
+      <c r="D17" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1296,18 +1441,18 @@
   <sheetData>
     <row r="3" spans="2:4" ht="32">
       <c r="C3" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="32">
       <c r="B6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>30</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="2:4">

</xml_diff>

<commit_message>
Cleaned comments in GUI. Made listOfNum wrap
</commit_message>
<xml_diff>
--- a/BoardGame/Stephanie.xlsx
+++ b/BoardGame/Stephanie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ng6739fk/Documents/GitHub/410/BoardGame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F813487A-17BB-A841-8090-129B65C2D54B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B9C85B-CE62-3146-9550-D806A01C9172}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="720" windowWidth="27020" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -142,9 +142,6 @@
     <t>4 hours sketching diagrams</t>
   </si>
   <si>
-    <t>32.0 hours</t>
-  </si>
-  <si>
     <t>10 times</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>Match</t>
   </si>
   <si>
-    <t>total 53 hours</t>
-  </si>
-  <si>
     <t>1 hours talking about it after testing</t>
   </si>
   <si>
@@ -203,6 +197,12 @@
   </si>
   <si>
     <t>Total time Spent (hours)</t>
+  </si>
+  <si>
+    <t>total 54 hours</t>
+  </si>
+  <si>
+    <t>33.0 hours</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1136,7 @@
   <dimension ref="B1:M17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1210,14 +1210,14 @@
         <v>29</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="10" t="s">
         <v>25</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1236,10 +1236,10 @@
         <v>7</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>36</v>
@@ -1248,13 +1248,13 @@
         <v>100</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J8" s="11">
         <v>24.25</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M8" s="11">
         <v>7.25</v>
@@ -1279,7 +1279,7 @@
         <v>37</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>36</v>
@@ -1288,13 +1288,13 @@
         <v>100</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J10" s="11">
         <v>8.75</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M10" s="11">
         <v>21.25</v>
@@ -1316,28 +1316,28 @@
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>36</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J12" s="11">
-        <v>11.25</v>
+        <v>12.25</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M12" s="11">
-        <v>11.25</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1365,16 +1365,16 @@
         <v>36</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J14" s="11">
         <v>5.75</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M14" s="11">
         <v>13.25</v>
@@ -1396,24 +1396,24 @@
         <v>11</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="G16" s="8">
         <v>100</v>
       </c>
       <c r="M16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="4:4" ht="16">
       <c r="D17" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>